<commit_message>
More work and just started accessibiilty
</commit_message>
<xml_diff>
--- a/report/flash-html-performance.xlsx
+++ b/report/flash-html-performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>IE9</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>Average flash</t>
+  </si>
+  <si>
+    <t>Average HTML5</t>
   </si>
 </sst>
 </file>
@@ -533,15 +539,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +570,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -577,8 +586,15 @@
         <f t="shared" ref="E2:E6" si="0">(C2+D2)/2</f>
         <v>0.95250000000000001</v>
       </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <f>(E1+E3+E5)/3</f>
+        <v>0.76666666666666661</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -597,8 +613,15 @@
         <f t="shared" si="0"/>
         <v>0.8175</v>
       </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <f>(E2+E4+E6)/3</f>
+        <v>0.87333333333333341</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -615,7 +638,7 @@
         <v>0.88749999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -635,7 +658,7 @@
         <v>0.86249999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>2</v>
       </c>

</xml_diff>